<commit_message>
Final version. For work you need- openpyxl
</commit_message>
<xml_diff>
--- a/ExcelDocument.xlsx
+++ b/ExcelDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Общая информация" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Вариант</t>
   </si>
@@ -205,15 +205,6 @@
   </si>
   <si>
     <t>Количество дней в году</t>
-  </si>
-  <si>
-    <t>Summa rasxodov</t>
-  </si>
-  <si>
-    <t>Года идут вниз</t>
-  </si>
-  <si>
-    <t>Зеленая - сумма</t>
   </si>
 </sst>
 </file>
@@ -397,13 +388,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -434,6 +422,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -744,15 +734,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="10"/>
+    <col min="7" max="7" width="8.85546875" style="7"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
@@ -782,10 +773,6 @@
       <c r="B3" s="1">
         <v>5</v>
       </c>
-      <c r="C3">
-        <f>20/5</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -794,10 +781,6 @@
       <c r="B4" s="1">
         <v>100</v>
       </c>
-      <c r="D4">
-        <f>B2/B3*1000</f>
-        <v>4000</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -808,10 +791,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="29">
         <v>0.14000000000000001</v>
       </c>
       <c r="I6">
@@ -834,15 +817,15 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="29">
         <v>0.11</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="29">
         <v>0.2</v>
       </c>
       <c r="H8" t="s">
@@ -870,10 +853,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -906,19 +889,19 @@
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="29">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="29">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="29">
         <v>3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="29">
         <v>4</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="29">
         <v>5</v>
       </c>
     </row>
@@ -926,20 +909,20 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="29">
         <f>0.7</f>
         <v>0.7</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="29">
         <v>0.9</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="29">
         <v>1</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="29">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="29">
         <v>0.8</v>
       </c>
       <c r="H12" t="s">
@@ -970,19 +953,19 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="30">
         <v>15</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="29">
         <v>6</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="29">
         <v>3</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="29">
         <v>2</v>
       </c>
     </row>
@@ -990,19 +973,19 @@
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="29">
         <v>0.2</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="29">
         <v>0.4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="29">
         <v>0.4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="29" t="s">
         <v>22</v>
       </c>
       <c r="H14" t="s">
@@ -1030,21 +1013,21 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <v>12</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="H16" s="12" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="H16" s="9" t="s">
         <v>41</v>
       </c>
       <c r="I16">
@@ -1067,16 +1050,16 @@
         <f>M14-M21+2000</f>
         <v>22048</v>
       </c>
-      <c r="N16" s="26"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1085,9 +1068,9 @@
       <c r="B18" s="1">
         <v>670</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1097,19 +1080,19 @@
         <f>B21+B22+B23</f>
         <v>460</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="H19" s="13" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="H19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="11">
         <v>1</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="11">
         <v>2</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1118,42 +1101,38 @@
         <v>1</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="H20" s="16" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="H20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="5">
         <f>((C2*1000)+I40)*(1+B7)</f>
         <v>14870.831875</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="5">
         <f>I22</f>
         <v>10717.716666666667</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="14">
         <f>J22</f>
         <v>5358.8583333333336</v>
       </c>
       <c r="L20">
-        <f>-1*(I40+20000)</f>
-        <v>-25397.145833333332</v>
+        <v>-21224.37</v>
       </c>
       <c r="M20">
-        <f>I26</f>
-        <v>8255.3577485380101</v>
+        <v>8451.0630000000001</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20:P20" si="5">J26</f>
-        <v>10859.460038986348</v>
+        <v>11613.27</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
-        <v>12074.790758829969</v>
+        <v>12856.05</v>
       </c>
       <c r="P20">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="N20:P20" si="5">L26</f>
         <v>13409.434121880047</v>
       </c>
       <c r="Q20">
@@ -1168,21 +1147,21 @@
       <c r="B21" s="1">
         <v>290</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="H21" s="16" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="H21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="5">
         <f>(((C2*1000)+I40)*0.2)+I23</f>
         <v>4153.1152083333336</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="5">
         <f>((C2*1000)+I40)*0.4+J23</f>
         <v>6537.8071666666674</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="14">
         <f>K20+K23</f>
         <v>5948.3327500000005</v>
       </c>
@@ -1194,21 +1173,21 @@
       <c r="B22" s="1">
         <v>110</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="H22" s="18" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="H22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="16">
         <f>I20-I21</f>
         <v>10717.716666666667</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="16">
         <f>((C2*1000)+I40)*0.4</f>
         <v>5358.8583333333336</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1219,12 +1198,10 @@
       <c r="B23" s="1">
         <v>60</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="H23" s="25" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="H23" s="22" t="s">
         <v>57</v>
       </c>
       <c r="I23">
@@ -1247,34 +1224,31 @@
       <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8">
-        <f>(B24+B25)*1000</f>
-        <v>9000</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="8" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="5">
         <f>I16*(1-$B$8)</f>
         <v>9411.1078333333335</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="5">
         <f t="shared" ref="J24:M24" si="6">J16*(1-$B$8)</f>
         <v>14112.954266666662</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="5">
         <f t="shared" si="6"/>
         <v>17889.333799999993</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="5">
         <f t="shared" si="6"/>
         <v>22647.999999999996</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="5">
         <f t="shared" si="6"/>
         <v>17638.400000000001</v>
       </c>
@@ -1286,25 +1260,25 @@
       <c r="B25" s="1">
         <v>4</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9" t="s">
         <v>32</v>
       </c>
       <c r="I26">
@@ -1335,16 +1309,16 @@
       <c r="B27" s="1">
         <v>19</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8">
-        <f>360/B27</f>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5">
+        <f>$B$32/B27</f>
         <v>18.94736842105263</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="11"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1353,38 +1327,38 @@
       <c r="B28" s="1">
         <v>20</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8">
-        <f t="shared" ref="E28:E31" si="8">360/B28</f>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5">
+        <f t="shared" ref="E28:E30" si="8">$B$32/B28</f>
         <v>18</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="21" t="s">
+      <c r="F28" s="5"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="18" t="s">
         <v>31</v>
       </c>
       <c r="I28">
         <f>I26+L20</f>
-        <v>-17141.78808479532</v>
+        <v>-12969.012251461989</v>
       </c>
       <c r="J28">
         <f>J26+I26+L20</f>
-        <v>-6282.3280458089757</v>
+        <v>-2109.5522124756426</v>
       </c>
       <c r="K28">
         <f>K26+I26+J26+L20</f>
-        <v>5792.4627130209956</v>
+        <v>9965.2385463543287</v>
       </c>
       <c r="L28">
         <f>L26+I26+J26+K26+L20</f>
-        <v>19201.896834901043</v>
+        <v>23374.672668234376</v>
       </c>
       <c r="M28">
         <f>M26+I26+J26+K26+L26+L20</f>
-        <v>28362.72908434521</v>
+        <v>32535.504917678543</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1394,18 +1368,18 @@
       <c r="B29" s="1">
         <v>5</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5">
         <f t="shared" si="8"/>
         <v>72</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1414,38 +1388,38 @@
       <c r="B30" s="1">
         <v>25</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5">
         <f t="shared" si="8"/>
         <v>14.4</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="22" t="s">
+      <c r="F30" s="5"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="5">
         <f>I28/(-1*$L$20)</f>
-        <v>-0.67494938987581066</v>
-      </c>
-      <c r="J30" s="8">
+        <v>-0.61104344917950404</v>
+      </c>
+      <c r="J30" s="5">
         <f t="shared" ref="J30:M30" si="9">J28/(-1*$L$20)</f>
-        <v>-0.24736354577149078</v>
-      </c>
-      <c r="K30" s="8">
+        <v>-9.9392924853630174E-2</v>
+      </c>
+      <c r="K30" s="5">
         <f t="shared" si="9"/>
-        <v>0.22807534165585192</v>
-      </c>
-      <c r="L30" s="8">
+        <v>0.46951869696741666</v>
+      </c>
+      <c r="L30" s="5">
         <f t="shared" si="9"/>
-        <v>0.75606514845848827</v>
-      </c>
-      <c r="M30" s="8">
+        <v>1.1013129090867892</v>
+      </c>
+      <c r="M30" s="5">
         <f t="shared" si="9"/>
-        <v>1.1167683672202093</v>
+        <v>1.5329314800711891</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1455,397 +1429,391 @@
       <c r="B31" s="1">
         <v>37</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="8">
-        <f t="shared" si="8"/>
+      <c r="E31" s="5">
+        <f>$B$32/B31</f>
         <v>9.7297297297297298</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>360</v>
       </c>
-      <c r="E32" s="25"/>
-      <c r="H32" s="21" t="s">
+      <c r="E32" s="22"/>
+      <c r="H32" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="20">
         <f>IRR(L20:Q20)</f>
-        <v>0.3007242636640437</v>
-      </c>
-    </row>
-    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H34" s="21" t="s">
+        <v>0.41623492718088628</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H34" s="18" t="s">
         <v>44</v>
       </c>
       <c r="I34">
         <f>$L$20+I24</f>
-        <v>-15986.037999999999</v>
+        <v>-11813.262166666666</v>
       </c>
       <c r="J34">
         <f>$L$20+J24+I24</f>
-        <v>-1873.0837333333366</v>
+        <v>2299.6920999999966</v>
       </c>
       <c r="K34">
         <f>$L$20+K24+I24+J24</f>
-        <v>16016.250066666656</v>
+        <v>20189.02589999999</v>
       </c>
       <c r="M34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H36" s="21" t="s">
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H36" s="18" t="s">
         <v>45</v>
       </c>
       <c r="I36">
         <f>$L$20+I26</f>
-        <v>-17141.78808479532</v>
+        <v>-12969.012251461989</v>
       </c>
       <c r="J36">
         <f>$L$20+J26+I26</f>
-        <v>-6282.3280458089739</v>
+        <v>-2109.5522124756408</v>
       </c>
       <c r="K36">
         <f>$L$20+K26+J26+I26</f>
-        <v>5792.4627130209956</v>
+        <v>9965.2385463543287</v>
       </c>
       <c r="L36">
         <f>$L$20+L26+K26+J26+I26</f>
-        <v>19201.896834901043</v>
+        <v>23374.672668234376</v>
       </c>
       <c r="M36" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H38" s="13" t="s">
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H38" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="K38" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L38" s="14" t="s">
+      <c r="L38" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M38" s="14" t="s">
+      <c r="M38" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="N38" s="15">
+      <c r="N38" s="12">
         <v>0</v>
       </c>
-      <c r="O38" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H39" s="16"/>
-      <c r="I39" s="8">
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H39" s="13"/>
+      <c r="I39" s="5">
         <f>($B$4*1000*B12*B21)/(360/B27)</f>
         <v>1071388.888888889</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="5">
         <f>($B$4*1000*B12*B19)/(360/$B28)</f>
         <v>1788888.888888889</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K39" s="5">
         <f>($B$4*1000*B12*B19)/(360/$B29)</f>
         <v>447222.22222222225</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L39" s="5">
         <f>I8/(360/$B30)</f>
         <v>3256.9444444444443</v>
       </c>
-      <c r="M39" s="8">
+      <c r="M39" s="5">
         <f>($B$4*1000*B12*B21)/(360/$B31)</f>
         <v>2086388.8888888888</v>
       </c>
-      <c r="N39" s="17"/>
-      <c r="O39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H40" s="16" t="s">
+      <c r="N39" s="14"/>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H40" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I40" s="28">
+      <c r="I40" s="25">
         <f>SUM(I39,J39,K39,L39,M39)/1000</f>
         <v>5397.145833333333</v>
       </c>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="29"/>
-    </row>
-    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="16"/>
-      <c r="I41" s="30">
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="26"/>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H41" s="13"/>
+      <c r="I41" s="27">
         <f>I42-I39</f>
         <v>306111.11111111101</v>
       </c>
-      <c r="J41" s="30">
+      <c r="J41" s="27">
         <f t="shared" ref="J41:M41" si="10">J42-J39</f>
         <v>511111.11111111101</v>
       </c>
-      <c r="K41" s="30">
+      <c r="K41" s="27">
         <f t="shared" si="10"/>
         <v>127777.77777777775</v>
       </c>
-      <c r="L41" s="30">
+      <c r="L41" s="27">
         <f t="shared" si="10"/>
         <v>930.55555555555566</v>
       </c>
-      <c r="M41" s="30">
+      <c r="M41" s="27">
         <f t="shared" si="10"/>
         <v>596111.11111111124</v>
       </c>
-      <c r="N41" s="31">
+      <c r="N41" s="28">
         <f>SUM(I41,J41,K41,L41,M41)/1000</f>
         <v>1542.0416666666665</v>
       </c>
     </row>
-    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H42" s="16"/>
-      <c r="I42" s="8">
+    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H42" s="13"/>
+      <c r="I42" s="5">
         <f>($B$4*1000*$C12*$B21)/$E27</f>
         <v>1377500</v>
       </c>
-      <c r="J42" s="8">
+      <c r="J42" s="5">
         <f>($B$4*1000*$C12*$B19)/$E28</f>
         <v>2300000</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K42" s="5">
         <f>($B$4*1000*$C12*$B19)/$E29</f>
         <v>575000</v>
       </c>
-      <c r="L42" s="8">
+      <c r="L42" s="5">
         <f>J8/$E30</f>
         <v>4187.5</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="5">
         <f>($B$4*1000*$C12*$B21)/$E31</f>
         <v>2682500</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N42" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H43" s="16"/>
-      <c r="I43" s="30">
+    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H43" s="13"/>
+      <c r="I43" s="27">
         <f>I44-I42</f>
         <v>153055.55555555574</v>
       </c>
-      <c r="J43" s="30">
+      <c r="J43" s="27">
         <f t="shared" ref="J43:M43" si="11">J44-J42</f>
         <v>255555.5555555555</v>
       </c>
-      <c r="K43" s="30">
+      <c r="K43" s="27">
         <f t="shared" si="11"/>
         <v>63888.888888888876</v>
       </c>
-      <c r="L43" s="30">
+      <c r="L43" s="27">
         <f t="shared" si="11"/>
         <v>465.27777777777737</v>
       </c>
-      <c r="M43" s="30">
+      <c r="M43" s="27">
         <f t="shared" si="11"/>
         <v>298055.5555555555</v>
       </c>
-      <c r="N43" s="31">
+      <c r="N43" s="28">
         <f>SUM(I43,J43,K43,L43,M43)/1000</f>
         <v>771.02083333333337</v>
       </c>
     </row>
-    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H44" s="16"/>
-      <c r="I44" s="8">
+    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H44" s="13"/>
+      <c r="I44" s="5">
         <f>($B$4*1000*$D$12*$B$21)/$E$27</f>
         <v>1530555.5555555557</v>
       </c>
-      <c r="J44" s="8">
+      <c r="J44" s="5">
         <f>($B$4*1000*$D$12*$B$19)/$E$28</f>
         <v>2555555.5555555555</v>
       </c>
-      <c r="K44" s="8">
+      <c r="K44" s="5">
         <f>($B$4*1000*$D$12*$B$19)/$E$29</f>
         <v>638888.88888888888</v>
       </c>
-      <c r="L44" s="8">
+      <c r="L44" s="5">
         <f>K8/$E$30</f>
         <v>4652.7777777777774</v>
       </c>
-      <c r="M44" s="8">
+      <c r="M44" s="5">
         <f>($B$4*1000*$D$12*$B$21)/$E$31</f>
         <v>2980555.5555555555</v>
       </c>
-      <c r="N44" s="17">
+      <c r="N44" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H45" s="16"/>
-      <c r="I45" s="30">
+    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H45" s="13"/>
+      <c r="I45" s="27">
         <v>0</v>
       </c>
-      <c r="J45" s="30">
+      <c r="J45" s="27">
         <v>0</v>
       </c>
-      <c r="K45" s="30">
+      <c r="K45" s="27">
         <v>0</v>
       </c>
-      <c r="L45" s="30">
+      <c r="L45" s="27">
         <v>0</v>
       </c>
-      <c r="M45" s="30">
+      <c r="M45" s="27">
         <v>0</v>
       </c>
-      <c r="N45" s="31">
+      <c r="N45" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H46" s="16"/>
-      <c r="I46" s="8">
+    <row r="46" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H46" s="13"/>
+      <c r="I46" s="5">
         <f>($B$4*1000*$E$12*$B$21)/$E$27</f>
         <v>1530555.5555555557</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="5">
         <f>($B$4*1000*$E$12*$B$19)/$E$28</f>
         <v>2555555.5555555555</v>
       </c>
-      <c r="K46" s="8">
+      <c r="K46" s="5">
         <f>($B$4*1000*$E$12*$B$19)/$E$29</f>
         <v>638888.88888888888</v>
       </c>
-      <c r="L46" s="8">
+      <c r="L46" s="5">
         <f>L8/$E$30</f>
         <v>4652.7777777777774</v>
       </c>
-      <c r="M46" s="8">
+      <c r="M46" s="5">
         <f>($B$4*1000*$E$12*$B$21)/$E$31</f>
         <v>2980555.5555555555</v>
       </c>
-      <c r="N46" s="17">
+      <c r="N46" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H47" s="16"/>
-      <c r="I47" s="30">
+    <row r="47" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H47" s="13"/>
+      <c r="I47" s="27">
         <f>I48-I46</f>
         <v>-306111.11111111124</v>
       </c>
-      <c r="J47" s="30">
+      <c r="J47" s="27">
         <f t="shared" ref="J47:M47" si="12">J48-J46</f>
         <v>-511111.11111111101</v>
       </c>
-      <c r="K47" s="30">
+      <c r="K47" s="27">
         <f t="shared" si="12"/>
         <v>-127777.77777777775</v>
       </c>
-      <c r="L47" s="30">
+      <c r="L47" s="27">
         <f t="shared" si="12"/>
         <v>-930.5555555555552</v>
       </c>
-      <c r="M47" s="30">
+      <c r="M47" s="27">
         <f t="shared" si="12"/>
         <v>-596111.11111111101</v>
       </c>
-      <c r="N47" s="31">
+      <c r="N47" s="28">
         <f>SUM(I47:M47)/1000</f>
         <v>-1542.0416666666665</v>
       </c>
     </row>
-    <row r="48" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H48" s="16"/>
-      <c r="I48" s="8">
+    <row r="48" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H48" s="13"/>
+      <c r="I48" s="5">
         <f>($B$4*1000*$F$12*$B$21)/$E$27</f>
         <v>1224444.4444444445</v>
       </c>
-      <c r="J48" s="8">
+      <c r="J48" s="5">
         <f>($B$4*1000*$F$12*$B$19)/$E$28</f>
         <v>2044444.4444444445</v>
       </c>
-      <c r="K48" s="8">
+      <c r="K48" s="5">
         <f>($B$4*1000*$F$12*$B$19)/$E$29</f>
         <v>511111.11111111112</v>
       </c>
-      <c r="L48" s="8">
+      <c r="L48" s="5">
         <f>M8/$E$30</f>
         <v>3722.2222222222222</v>
       </c>
-      <c r="M48" s="8">
+      <c r="M48" s="5">
         <f>($B$4*1000*$F$12*$B$21)/$E$31</f>
         <v>2384444.4444444445</v>
       </c>
-      <c r="N48" s="17">
+      <c r="N48" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H49" s="16"/>
-      <c r="I49" s="30">
+      <c r="H49" s="13"/>
+      <c r="I49" s="27">
         <f>I50-I48</f>
         <v>-1224444.4444444445</v>
       </c>
-      <c r="J49" s="30">
+      <c r="J49" s="27">
         <f t="shared" ref="J49:M49" si="13">J50-J48</f>
         <v>-2044444.4444444445</v>
       </c>
-      <c r="K49" s="30">
+      <c r="K49" s="27">
         <f t="shared" si="13"/>
         <v>-511111.11111111112</v>
       </c>
-      <c r="L49" s="30">
+      <c r="L49" s="27">
         <f t="shared" si="13"/>
         <v>-3722.2222222222222</v>
       </c>
-      <c r="M49" s="30">
+      <c r="M49" s="27">
         <f t="shared" si="13"/>
         <v>-2384444.4444444445</v>
       </c>
-      <c r="N49" s="31">
+      <c r="N49" s="28">
         <f>SUM(I49:M49)/1000</f>
         <v>-6168.1666666666661</v>
       </c>
     </row>
     <row r="50" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H50" s="18"/>
-      <c r="I50" s="19">
+      <c r="H50" s="15"/>
+      <c r="I50" s="16">
         <v>0</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50" s="16">
         <v>0</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="16">
         <v>0</v>
       </c>
-      <c r="L50" s="19">
+      <c r="L50" s="16">
         <v>0</v>
       </c>
-      <c r="M50" s="19">
+      <c r="M50" s="16">
         <v>0</v>
       </c>
-      <c r="N50" s="20">
+      <c r="N50" s="17">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H54" s="27" t="s">
+      <c r="H54" s="24" t="s">
         <v>61</v>
       </c>
       <c r="I54">
@@ -1889,105 +1857,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>2</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="6">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="6">
         <v>7</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="6">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="6">
         <v>9</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="6">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="6">
         <v>11</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="6">
         <v>13</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="6">
         <v>14</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="6">
         <v>15</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="6">
         <v>16</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="6">
         <v>17</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="6">
         <v>18</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="6">
         <v>19</v>
       </c>
-      <c r="U2" s="9">
+      <c r="U2" s="6">
         <v>20</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="6">
         <v>21</v>
       </c>
-      <c r="W2" s="9">
+      <c r="W2" s="6">
         <v>22</v>
       </c>
-      <c r="X2" s="9">
+      <c r="X2" s="6">
         <v>23</v>
       </c>
-      <c r="Y2" s="9">
+      <c r="Y2" s="6">
         <v>24</v>
       </c>
-      <c r="Z2" s="9">
+      <c r="Z2" s="6">
         <v>25</v>
       </c>
     </row>
@@ -3004,7 +2972,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>